<commit_message>
New home page & fix dahsboard page
</commit_message>
<xml_diff>
--- a/Changelog.xlsx
+++ b/Changelog.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ehsan\Desktop\project\pishgam_website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6E75E2-E61D-4E53-B6BA-4A088270EA51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF86D26-360D-4C3F-8219-537692BA72E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="master" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">master!$B$3:$F$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,20 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>تاریخ</t>
   </si>
   <si>
-    <t>فرد تغییر دهنده</t>
-  </si>
-  <si>
-    <t>توضیحات تکمیلی</t>
-  </si>
-  <si>
-    <t>تیتر تغییر</t>
-  </si>
-  <si>
     <t>لیست تغییرات پروژه ی کلاس آنلاین</t>
   </si>
   <si>
@@ -64,15 +55,32 @@
   </si>
   <si>
     <t>افراد پروژه</t>
+  </si>
+  <si>
+    <t>تیتر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فرد </t>
+  </si>
+  <si>
+    <t>توضیحات</t>
+  </si>
+  <si>
+    <t>بک / فرانت</t>
+  </si>
+  <si>
+    <t>بک اند</t>
+  </si>
+  <si>
+    <t>فرانت اند</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-160429]dd/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-960429]dd/mm/yyyy;@"/>
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="[$-960429]dddd\,\ d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -244,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -253,32 +261,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -311,6 +298,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,106 +602,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H11"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="32.1796875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="16" style="8" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="54.26953125" style="15" customWidth="1"/>
-    <col min="6" max="7" width="8.7265625" style="2"/>
-    <col min="8" max="9" width="18.26953125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="32.1796875" style="12" customWidth="1"/>
+    <col min="3" max="4" width="16" style="5" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" style="22" customWidth="1"/>
+    <col min="6" max="6" width="54.26953125" style="8" customWidth="1"/>
+    <col min="7" max="8" width="8.7265625" style="2"/>
+    <col min="9" max="10" width="18.26953125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="B1" s="16"/>
+    <row r="1" spans="2:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="B1" s="9"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="1"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="2:8" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="B2" s="4" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="1"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="2:10" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="B2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="2:10" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="B3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="35" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="B4" s="11"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="21">
+        <v>41356</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="I4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="E5" s="22">
+        <v>41355</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="E6" s="22">
+        <v>41724</v>
+      </c>
+      <c r="I6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="2:8" ht="35" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.8">
-      <c r="B3" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="B4" s="18"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="14"/>
-      <c r="H4" s="22" t="s">
+    </row>
+    <row r="7" spans="2:10" ht="35" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I7" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="H5" s="22" t="s">
+    <row r="8" spans="2:10" ht="35" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I8" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="H6" s="22" t="s">
+    <row r="9" spans="2:10" ht="35" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I9" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="H7" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="H8" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="H9" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="H11" s="23"/>
+    <row r="10" spans="2:10" ht="35" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="2:10" ht="35" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="I11" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E4" xr:uid="{9F481FE2-CE95-49B6-B418-8D07148DA2B8}"/>
+  <autoFilter ref="B3:F6" xr:uid="{9F481FE2-CE95-49B6-B418-8D07148DA2B8}">
+    <filterColumn colId="3">
+      <filters calendarType="none">
+        <dateGroupItem year="1393" dateTimeGrouping="year"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="شخص مورد نظر" sqref="C4:C8" xr:uid="{A2D9F7A4-7D1C-4265-974C-B4EA967C1AB9}">
-      <formula1>$H$4:$H$9</formula1>
+      <formula1>$I$4:$I$9</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="شخص مورد نظر" sqref="D4:D1048576" xr:uid="{AF8E5DEE-2A8A-4723-B976-4A2E684FE143}">
+      <formula1>$J$4:$J$5</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="شخص مورد نظر" sqref="D3 B2:F2 D1" xr:uid="{1513CB0F-7DDB-4FD7-9469-A1DA94D95619}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>